<commit_message>
Finalizing consensus doc + links added across the board.
</commit_message>
<xml_diff>
--- a/source/FullNode/Consensus/tables/Components.xlsx
+++ b/source/FullNode/Consensus/tables/Components.xlsx
@@ -2,18 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr checkCompatibility="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jtopham/Documents/Stratis/Academy/Documentation/source/FullNode/Consensus/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1028A57C-9610-3449-9718-53770184B542}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0377446B-E3DE-F148-BEDD-52DDF9FBAEA7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5200" yWindow="3560" windowWidth="28040" windowHeight="17440" xr2:uid="{4F4E2000-911A-A449-8EC7-F6920D0537F4}"/>
+    <workbookView xWindow="820" yWindow="1220" windowWidth="28040" windowHeight="17440" xr2:uid="{4F4E2000-911A-A449-8EC7-F6920D0537F4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Components" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>PoW Mining</t>
   </si>
@@ -43,6 +43,129 @@
   </si>
   <si>
     <t>`IPosMinting &lt;https://github.com/stratisproject/StratisBitcoinFullNode/blob/master/src/Stratis.Bitcoin.Features.Miner/Interfaces/IPosMinting.cs&gt;`_</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>C# Class</t>
+  </si>
+  <si>
+    <t>C# Interface</t>
+  </si>
+  <si>
+    <t>PoA Miner</t>
+  </si>
+  <si>
+    <t>Chained Header Tree</t>
+  </si>
+  <si>
+    <t>Consensus Manager</t>
+  </si>
+  <si>
+    <t>Consensus Manager Behavior</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Header Validator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrity Validator </t>
+  </si>
+  <si>
+    <t>Partial Validator</t>
+  </si>
+  <si>
+    <t>Full Validator</t>
+  </si>
+  <si>
+    <t>Consensus Rule Engine</t>
+  </si>
+  <si>
+    <t>PoW Consensus Rule Engine</t>
+  </si>
+  <si>
+    <t>PoS Consensus Rule Engine</t>
+  </si>
+  <si>
+    <t>PoA Consensus Rule Engine</t>
+  </si>
+  <si>
+    <t>Block Puller</t>
+  </si>
+  <si>
+    <t>`HeaderValidator &lt;https://github.com/stratisproject/StratisBitcoinFullNode/blob/master/src/Stratis.Bitcoin/Consensus/Validators/BlockValidator.cs&gt;`_</t>
+  </si>
+  <si>
+    <t>`IntegrityValidator &lt;https://github.com/stratisproject/StratisBitcoinFullNode/blob/master/src/Stratis.Bitcoin/Consensus/Validators/BlockValidator.cs&gt;`_</t>
+  </si>
+  <si>
+    <t>`PartialValidator  &lt;https://github.com/stratisproject/StratisBitcoinFullNode/blob/master/src/Stratis.Bitcoin/Consensus/Validators/BlockValidator.cs&gt;`_</t>
+  </si>
+  <si>
+    <t>`FullValidator  &lt;https://github.com/stratisproject/StratisBitcoinFullNode/blob/master/src/Stratis.Bitcoin/Consensus/Validators/BlockValidator.cs&gt;`_</t>
+  </si>
+  <si>
+    <t>`IHeaderValidator  &lt;https://github.com/stratisproject/StratisBitcoinFullNode/blob/master/src/Stratis.Bitcoin/Consensus/Validators/BlockValidator.cs&gt;`_</t>
+  </si>
+  <si>
+    <t>`IIntegrity Validator  &lt;https://github.com/stratisproject/StratisBitcoinFullNode/blob/master/src/Stratis.Bitcoin/Consensus/Validators/BlockValidator.cs&gt;`_</t>
+  </si>
+  <si>
+    <t>`IPartialValidator  &lt;https://github.com/stratisproject/StratisBitcoinFullNode/blob/master/src/Stratis.Bitcoin/Consensus/Validators/BlockValidator.cs&gt;`_</t>
+  </si>
+  <si>
+    <t>`IFullValidator &lt;https://github.com/stratisproject/StratisBitcoinFullNode/blob/master/src/Stratis.Bitcoin/Consensus/Validators/BlockValidator.cs&gt;`_</t>
+  </si>
+  <si>
+    <t>Block Puller Behavior</t>
+  </si>
+  <si>
+    <t>`PoAMiner &lt;https://github.com/stratisproject/StratisBitcoinFullNode/blob/master/src/Stratis.Bitcoin.Features.PoA/PoAMiner.cs&gt;`_</t>
+  </si>
+  <si>
+    <t>`IPoAMiner &lt;https://github.com/stratisproject/StratisBitcoinFullNode/blob/master/src/Stratis.Bitcoin.Features.PoA/PoAMiner.cs&gt;`_</t>
+  </si>
+  <si>
+    <t>`ChainedHeaderTree &lt;https://github.com/stratisproject/StratisBitcoinFullNode/blob/master/src/Stratis.Bitcoin/Consensus/ChainedHeaderTree.cs&gt;'_</t>
+  </si>
+  <si>
+    <t>`IChainedHeaderTree &lt;https://github.com/stratisproject/StratisBitcoinFullNode/blob/master/src/Stratis.Bitcoin/Consensus/ChainedHeaderTree.cs&gt;'_</t>
+  </si>
+  <si>
+    <t>`ConsensusManager &lt;https://github.com/stratisproject/StratisBitcoinFullNode/blob/master/src/Stratis.Bitcoin/Consensus/ConsensusManager.cs&gt;`_</t>
+  </si>
+  <si>
+    <t>`IConsensusManager &lt;https://github.com/stratisproject/StratisBitcoinFullNode/blob/master/src/Stratis.Bitcoin/Consensus/IConsensusManager.cs&gt;`_</t>
+  </si>
+  <si>
+    <t>`Consensus Manager Behavior &lt;https://github.com/stratisproject/StratisBitcoinFullNode/blob/master/src/Stratis.Bitcoin/Consensus/ConsensusManagerBehavior.cs&gt;`_</t>
+  </si>
+  <si>
+    <t>`ConsensusRuleEngine &lt;https://github.com/stratisproject/StratisBitcoinFullNode/blob/master/src/Stratis.Bitcoin/Consensus/ConsensusManagerBehavior.cs&gt;`_</t>
+  </si>
+  <si>
+    <t>`IConsensusRuleEngine &lt;https://github.com/stratisproject/StratisBitcoinFullNode/blob/master/src/Stratis.Bitcoin/Consensus/IConsensusManagerBehavior.cs&gt;`_</t>
+  </si>
+  <si>
+    <t>`BlockPuller &lt;https://github.com/stratisproject/StratisBitcoinFullNode/blob/master/src/Stratis.Bitcoin/BlockPulling/BlockPuller.cs&gt;`_</t>
+  </si>
+  <si>
+    <t>`IBlockPuller &lt;https://github.com/stratisproject/StratisBitcoinFullNode/blob/master/src/Stratis.Bitcoin/BlockPulling/IBlockPuller.cs&gt;`_</t>
+  </si>
+  <si>
+    <t>`BlockPullerBehavior &lt;https://github.com/stratisproject/StratisBitcoinFullNode/blob/master/src/Stratis.Bitcoin/BlockPulling/BlockPullerBehavior.cs&gt;`_</t>
+  </si>
+  <si>
+    <t>`PowConsensusRuleEngine &lt;https://github.com/stratisproject/StratisBitcoinFullNode/blob/master/src/Stratis.Bitcoin.Features.Consensus/Rules/PowConsensusRuleEngine.cs&gt;`_</t>
+  </si>
+  <si>
+    <t>`PosConsensusRuleEngine &lt;https://github.com/stratisproject/StratisBitcoinFullNode/blob/master/src/Stratis.Bitcoin.Features.Consensus/Rules/PosConsensusRuleEngine.cs&gt;`</t>
+  </si>
+  <si>
+    <t>`PoAConsensusRuleEngine &lt;https://github.com/stratisproject/StratisBitcoinFullNode/blob/master/src/Stratis.Bitcoin.Features.PoA/PoAConsensusRuleEngine.cs&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -78,8 +201,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,34 +518,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D10FA63B-1713-C946-A020-191F04FC0D28}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="51.83203125" customWidth="1"/>
+    <col min="2" max="2" width="145.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>